<commit_message>
time added for students to appear for test
</commit_message>
<xml_diff>
--- a/DOCUMENT/Old_Docs/allowed_enrolls.xlsx
+++ b/DOCUMENT/Old_Docs/allowed_enrolls.xlsx
@@ -20,9 +20,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t xml:space="preserve">ENROLLMENT_NUMBER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YEAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MONTH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DATE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">START_TIME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">END_TIME</t>
   </si>
   <si>
     <t xml:space="preserve">19bt04001</t>
@@ -146,8 +161,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="hh:mm:ss"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -268,8 +284,8 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -349,14 +365,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A62"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A41" activeCellId="0" sqref="A41:A62"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2:F40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1020" style="0" width="9.14"/>
   </cols>
   <sheetData>
@@ -364,272 +383,806 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="E2" s="3" t="n">
+        <v>0.0194444444444444</v>
+      </c>
+      <c r="F2" s="3" t="n">
+        <v>0.0208333333333333</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>7</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="E3" s="3" t="n">
+        <v>0.0194444444444444</v>
+      </c>
+      <c r="F3" s="3" t="n">
+        <v>0.0208333333333333</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>3</v>
+        <v>8</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="E4" s="3" t="n">
+        <v>0.0194444444444444</v>
+      </c>
+      <c r="F4" s="3" t="n">
+        <v>0.0208333333333333</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>4</v>
+        <v>9</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="E5" s="3" t="n">
+        <v>0.0194444444444444</v>
+      </c>
+      <c r="F5" s="3" t="n">
+        <v>0.0208333333333333</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>5</v>
+        <v>10</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="E6" s="3" t="n">
+        <v>0.0194444444444444</v>
+      </c>
+      <c r="F6" s="3" t="n">
+        <v>0.0208333333333333</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>6</v>
+        <v>11</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="E7" s="3" t="n">
+        <v>0.0194444444444444</v>
+      </c>
+      <c r="F7" s="3" t="n">
+        <v>0.0208333333333333</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>7</v>
+        <v>12</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="E8" s="3" t="n">
+        <v>0.0194444444444444</v>
+      </c>
+      <c r="F8" s="3" t="n">
+        <v>0.0208333333333333</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="E9" s="3" t="n">
+        <v>0.0194444444444444</v>
+      </c>
+      <c r="F9" s="3" t="n">
+        <v>0.0208333333333333</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="E10" s="3" t="n">
+        <v>0.0194444444444444</v>
+      </c>
+      <c r="F10" s="3" t="n">
+        <v>0.0208333333333333</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>10</v>
+        <v>15</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="E11" s="3" t="n">
+        <v>0.0194444444444444</v>
+      </c>
+      <c r="F11" s="3" t="n">
+        <v>0.0208333333333333</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>11</v>
+        <v>16</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="E12" s="3" t="n">
+        <v>0.0194444444444444</v>
+      </c>
+      <c r="F12" s="3" t="n">
+        <v>0.0208333333333333</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>12</v>
+        <v>17</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="E13" s="3" t="n">
+        <v>0.0194444444444444</v>
+      </c>
+      <c r="F13" s="3" t="n">
+        <v>0.0208333333333333</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>13</v>
+        <v>18</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="E14" s="3" t="n">
+        <v>0.0194444444444444</v>
+      </c>
+      <c r="F14" s="3" t="n">
+        <v>0.0208333333333333</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>14</v>
+        <v>19</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="E15" s="3" t="n">
+        <v>0.0194444444444444</v>
+      </c>
+      <c r="F15" s="3" t="n">
+        <v>0.0208333333333333</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>15</v>
+        <v>20</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="E16" s="3" t="n">
+        <v>0.0194444444444444</v>
+      </c>
+      <c r="F16" s="3" t="n">
+        <v>0.0208333333333333</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>16</v>
+        <v>21</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="E17" s="3" t="n">
+        <v>0.0194444444444444</v>
+      </c>
+      <c r="F17" s="3" t="n">
+        <v>0.0208333333333333</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>17</v>
+        <v>22</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="E18" s="3" t="n">
+        <v>0.0194444444444444</v>
+      </c>
+      <c r="F18" s="3" t="n">
+        <v>0.0208333333333333</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>18</v>
+        <v>23</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="E19" s="3" t="n">
+        <v>0.0194444444444444</v>
+      </c>
+      <c r="F19" s="3" t="n">
+        <v>0.0208333333333333</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>19</v>
+        <v>24</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="E20" s="3" t="n">
+        <v>0.0194444444444444</v>
+      </c>
+      <c r="F20" s="3" t="n">
+        <v>0.0208333333333333</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>20</v>
+        <v>25</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="E21" s="3" t="n">
+        <v>0.0194444444444444</v>
+      </c>
+      <c r="F21" s="3" t="n">
+        <v>0.0208333333333333</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>21</v>
+        <v>26</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="E22" s="3" t="n">
+        <v>0.0194444444444444</v>
+      </c>
+      <c r="F22" s="3" t="n">
+        <v>0.0208333333333333</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>22</v>
+        <v>27</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="E23" s="3" t="n">
+        <v>0.0194444444444444</v>
+      </c>
+      <c r="F23" s="3" t="n">
+        <v>0.0208333333333333</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>23</v>
+        <v>28</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="E24" s="3" t="n">
+        <v>0.0194444444444444</v>
+      </c>
+      <c r="F24" s="3" t="n">
+        <v>0.0208333333333333</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>24</v>
+        <v>29</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="E25" s="3" t="n">
+        <v>0.0194444444444444</v>
+      </c>
+      <c r="F25" s="3" t="n">
+        <v>0.0208333333333333</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>25</v>
+        <v>30</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="E26" s="3" t="n">
+        <v>0.0194444444444444</v>
+      </c>
+      <c r="F26" s="3" t="n">
+        <v>0.0208333333333333</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="E27" s="3" t="n">
+        <v>0.0194444444444444</v>
+      </c>
+      <c r="F27" s="3" t="n">
+        <v>0.0208333333333333</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
-        <v>27</v>
+        <v>32</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="E28" s="3" t="n">
+        <v>0.0194444444444444</v>
+      </c>
+      <c r="F28" s="3" t="n">
+        <v>0.0208333333333333</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
-        <v>28</v>
+        <v>33</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D29" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="E29" s="3" t="n">
+        <v>0.0194444444444444</v>
+      </c>
+      <c r="F29" s="3" t="n">
+        <v>0.0208333333333333</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
-        <v>29</v>
+        <v>34</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D30" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="E30" s="3" t="n">
+        <v>0.0194444444444444</v>
+      </c>
+      <c r="F30" s="3" t="n">
+        <v>0.0208333333333333</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
-        <v>30</v>
+        <v>35</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C31" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D31" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="E31" s="3" t="n">
+        <v>0.0194444444444444</v>
+      </c>
+      <c r="F31" s="3" t="n">
+        <v>0.0208333333333333</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
-        <v>31</v>
+        <v>36</v>
+      </c>
+      <c r="B32" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C32" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D32" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="E32" s="3" t="n">
+        <v>0.0194444444444444</v>
+      </c>
+      <c r="F32" s="3" t="n">
+        <v>0.0208333333333333</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
-        <v>32</v>
+        <v>37</v>
+      </c>
+      <c r="B33" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C33" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D33" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="E33" s="3" t="n">
+        <v>0.0194444444444444</v>
+      </c>
+      <c r="F33" s="3" t="n">
+        <v>0.0208333333333333</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
-        <v>33</v>
+        <v>38</v>
+      </c>
+      <c r="B34" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C34" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D34" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="E34" s="3" t="n">
+        <v>0.0194444444444444</v>
+      </c>
+      <c r="F34" s="3" t="n">
+        <v>0.0208333333333333</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
-        <v>34</v>
+        <v>39</v>
+      </c>
+      <c r="B35" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C35" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D35" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="E35" s="3" t="n">
+        <v>0.0194444444444444</v>
+      </c>
+      <c r="F35" s="3" t="n">
+        <v>0.0208333333333333</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
-        <v>35</v>
+        <v>40</v>
+      </c>
+      <c r="B36" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C36" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D36" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="E36" s="3" t="n">
+        <v>0.0194444444444444</v>
+      </c>
+      <c r="F36" s="3" t="n">
+        <v>0.0208333333333333</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="s">
-        <v>36</v>
+        <v>41</v>
+      </c>
+      <c r="B37" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C37" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D37" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="E37" s="3" t="n">
+        <v>0.0194444444444444</v>
+      </c>
+      <c r="F37" s="3" t="n">
+        <v>0.0208333333333333</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
-        <v>37</v>
+        <v>42</v>
+      </c>
+      <c r="B38" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C38" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D38" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="E38" s="3" t="n">
+        <v>0.0194444444444444</v>
+      </c>
+      <c r="F38" s="3" t="n">
+        <v>0.0208333333333333</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="s">
-        <v>38</v>
+        <v>43</v>
+      </c>
+      <c r="B39" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C39" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D39" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="E39" s="3" t="n">
+        <v>0.0194444444444444</v>
+      </c>
+      <c r="F39" s="3" t="n">
+        <v>0.0208333333333333</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="2"/>
-    </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="2"/>
-    </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="2"/>
-    </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="2"/>
-    </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="2"/>
-    </row>
-    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="2"/>
-    </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="2"/>
-    </row>
-    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="2"/>
-    </row>
-    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="2"/>
-    </row>
-    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="2"/>
-    </row>
-    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="2"/>
-    </row>
-    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="2"/>
-    </row>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="2"/>
-    </row>
-    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="2"/>
-    </row>
-    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="2"/>
-    </row>
-    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="2"/>
-    </row>
-    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="2"/>
-    </row>
-    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="2"/>
-    </row>
-    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="3"/>
-    </row>
-    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="3"/>
-    </row>
-    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="3"/>
-    </row>
-    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="3"/>
+        <v>44</v>
+      </c>
+      <c r="B40" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C40" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D40" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="E40" s="3" t="n">
+        <v>0.0194444444444444</v>
+      </c>
+      <c r="F40" s="3" t="n">
+        <v>0.0208333333333333</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>